<commit_message>
quiz eco1.json change in vscode
</commit_message>
<xml_diff>
--- a/files/PSkabelon.xlsx
+++ b/files/PSkabelon.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomaspetersen/Documents/GitHub/jekyll-unicorn/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{300BFC9C-1C38-3241-A9A6-CF68D7053DB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0486E2DB-9FAE-CC45-8128-A870A819BCE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="88">
   <si>
     <t>Tidshorisont</t>
   </si>
@@ -309,22 +309,7 @@
     <t>Hvis blank max kap A8</t>
   </si>
   <si>
-    <t>mini</t>
-  </si>
-  <si>
-    <t>nivi</t>
-  </si>
-  <si>
-    <t>emma</t>
-  </si>
-  <si>
-    <t>tina</t>
-  </si>
-  <si>
-    <t>arnaminaq</t>
-  </si>
-  <si>
-    <t>pilo</t>
+    <t>Elasticitet</t>
   </si>
 </sst>
 </file>
@@ -774,7 +759,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>P = -1·Q + 80</c:v>
+                  <c:v>P = -1·Q + 100</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -855,7 +840,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>80</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -867,7 +852,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>80</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -891,7 +876,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Pris = 50</c:v>
+                  <c:v>Pris = 50kr. Elasticiteten er -1. Når prisen sænkes med 1%, stiger afsætningen med 1%. Efterspørgslen er neutralelastisk</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -973,7 +958,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>30</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1009,7 +994,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Mængde = 30</c:v>
+                  <c:v>Mængde = 50</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1088,10 +1073,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>30</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>30</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1127,7 +1112,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>OMSÆTNING = 50*30=1500</c:v>
+                  <c:v>OMSÆTNING = 50*50=2500</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1165,11 +1150,11 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>P!$A$91</c:f>
+              <c:f>P!$A$90</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Markedsmætning = 80 Q</c:v>
+                  <c:v>Markedsmætning = 100 Q</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1237,7 +1222,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>80</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1270,7 +1255,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Maks. betalingsvillighed = 80 kr.</c:v>
+                  <c:v>Maks. betalingsvillighed = 100 kr.</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1364,7 +1349,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>80</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1385,7 +1370,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Maks. omsætning = 40*40 = 1600 kr.</c:v>
+                  <c:v>Maks. omsætning = 50*50 = 2500 kr.</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1432,6 +1417,7 @@
                 <a:endParaRPr lang="da-DK"/>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="l"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1452,7 +1438,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>40</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1464,7 +1450,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>40</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1727,8 +1713,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.77857020776768748"/>
           <c:y val="9.7487483708669109E-2"/>
-          <c:w val="0.16970482271577256"/>
-          <c:h val="0.22888683223070214"/>
+          <c:w val="0.16921174010291917"/>
+          <c:h val="0.23203806159333426"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -1881,7 +1867,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>P = -0,01·m + 2000</c:v>
+                  <c:v>P = -0,02·m + 300</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1962,7 +1948,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>200000</c:v>
+                  <c:v>15000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1974,7 +1960,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>2000</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -1998,7 +1984,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>GROMS = -0,02·m + 2000</c:v>
+                  <c:v>GROMS = -0,04·m + 300</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2079,7 +2065,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100000</c:v>
+                  <c:v>7500</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2091,7 +2077,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>2000</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -2115,7 +2101,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>GROMK = </c:v>
+                  <c:v>GROMK = 0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2196,7 +2182,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>200000</c:v>
+                  <c:v>15000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2336,7 +2322,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Optimal pris = 1000</c:v>
+                  <c:v>Optimal pris = 150</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2418,7 +2404,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100000</c:v>
+                  <c:v>7500</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2430,10 +2416,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>1000</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1000</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2454,7 +2440,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Optimal mængde = 100000</c:v>
+                  <c:v>Optimal mængde = 7500</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2534,10 +2520,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>100000</c:v>
+                  <c:v>7500</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100000</c:v>
+                  <c:v>7500</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2552,7 +2538,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1000</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2573,7 +2559,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>VE = </c:v>
+                  <c:v>VE = 0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2656,7 +2642,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>200000</c:v>
+                  <c:v>15000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2692,7 +2678,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>OMSÆTNING = 100000000</c:v>
+                  <c:v>OMSÆTNING = 1125000</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2778,7 +2764,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>DB = 100000000</c:v>
+                  <c:v>DB = 1125000</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -8523,10 +8509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B603048-6EF1-724D-8231-2F202BA806A1}">
-  <dimension ref="A1:Q110"/>
+  <dimension ref="A1:M110"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="136" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" zoomScale="137" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8554,7 +8540,7 @@
         <v>-1</v>
       </c>
       <c r="B3" s="62">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="E3" s="37"/>
     </row>
@@ -8605,121 +8591,103 @@
     <row r="16" spans="1:5" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E16" s="42"/>
     </row>
-    <row r="17" spans="5:17" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="5:5" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E17" s="42"/>
     </row>
-    <row r="18" spans="5:17" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="5:5" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E18" s="42"/>
     </row>
-    <row r="19" spans="5:17" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="5:5" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E19" s="42"/>
     </row>
-    <row r="20" spans="5:17" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="5:5" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E20" s="42"/>
     </row>
-    <row r="21" spans="5:17" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="5:5" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E21" s="42"/>
     </row>
-    <row r="22" spans="5:17" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="5:5" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E22" s="42"/>
     </row>
-    <row r="23" spans="5:17" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="5:5" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E23" s="42"/>
     </row>
-    <row r="24" spans="5:17" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="5:5" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E24" s="42"/>
     </row>
-    <row r="25" spans="5:17" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="5:5" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E25" s="42"/>
     </row>
-    <row r="26" spans="5:17" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="5:5" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E26" s="42"/>
     </row>
-    <row r="27" spans="5:17" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="5:5" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E27" s="42"/>
     </row>
-    <row r="28" spans="5:17" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="5:5" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E28" s="42"/>
     </row>
-    <row r="29" spans="5:17" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="5:5" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E29" s="42"/>
-      <c r="Q29" s="34" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="30" spans="5:17" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="5:5" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E30" s="42"/>
-      <c r="Q30" s="34" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="31" spans="5:17" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="5:5" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E31" s="42"/>
-      <c r="Q31" s="34" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="32" spans="5:17" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="5:5" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E32" s="42"/>
-      <c r="Q32" s="34" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="33" spans="5:17" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="5:5" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E33" s="42"/>
-      <c r="Q33" s="34" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="34" spans="5:17" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="5:5" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E34" s="42"/>
-      <c r="Q34" s="34" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="35" spans="5:17" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="5:5" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E35" s="42"/>
     </row>
-    <row r="36" spans="5:17" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="5:5" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E36" s="42"/>
     </row>
-    <row r="37" spans="5:17" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="5:5" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E37" s="42"/>
     </row>
-    <row r="38" spans="5:17" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="5:5" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E38" s="42"/>
     </row>
-    <row r="39" spans="5:17" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="5:5" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E39" s="42"/>
     </row>
-    <row r="40" spans="5:17" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="5:5" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E40" s="42"/>
     </row>
-    <row r="41" spans="5:17" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="5:5" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E41" s="42"/>
     </row>
-    <row r="42" spans="5:17" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="5:5" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E42" s="42"/>
     </row>
-    <row r="43" spans="5:17" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="5:5" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E43" s="42"/>
     </row>
-    <row r="44" spans="5:17" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="5:5" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E44" s="42"/>
     </row>
-    <row r="45" spans="5:17" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="5:5" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E45" s="42"/>
     </row>
-    <row r="46" spans="5:17" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="5:5" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E46" s="42"/>
     </row>
-    <row r="47" spans="5:17" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="5:5" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E47" s="42"/>
     </row>
-    <row r="48" spans="5:17" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="5:5" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E48" s="42"/>
     </row>
-    <row r="49" spans="1:10" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:13" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="44"/>
       <c r="B49" s="44"/>
       <c r="C49" s="44"/>
@@ -8731,7 +8699,7 @@
       <c r="I49" s="44"/>
       <c r="J49" s="44"/>
     </row>
-    <row r="50" spans="1:10" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:13" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="44"/>
       <c r="B50" s="44"/>
       <c r="C50" s="44"/>
@@ -8743,7 +8711,7 @@
       <c r="I50" s="44"/>
       <c r="J50" s="44"/>
     </row>
-    <row r="51" spans="1:10" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:13" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="44"/>
       <c r="B51" s="44"/>
       <c r="C51" s="44"/>
@@ -8755,7 +8723,7 @@
       <c r="I51" s="44"/>
       <c r="J51" s="44"/>
     </row>
-    <row r="52" spans="1:10" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:13" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="44"/>
       <c r="B52" s="44"/>
       <c r="C52" s="44"/>
@@ -8767,7 +8735,7 @@
       <c r="I52" s="44"/>
       <c r="J52" s="44"/>
     </row>
-    <row r="53" spans="1:10" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:13" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="44"/>
       <c r="B53" s="44"/>
       <c r="C53" s="44"/>
@@ -8779,7 +8747,7 @@
       <c r="I53" s="44"/>
       <c r="J53" s="44"/>
     </row>
-    <row r="54" spans="1:10" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:13" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A54" s="44"/>
       <c r="B54" s="44"/>
       <c r="C54" s="44"/>
@@ -8791,7 +8759,7 @@
       <c r="I54" s="44"/>
       <c r="J54" s="44"/>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55" s="44"/>
       <c r="B55" s="44"/>
       <c r="C55" s="36"/>
@@ -8803,7 +8771,7 @@
       <c r="I55" s="36"/>
       <c r="J55" s="36"/>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56" s="44"/>
       <c r="B56" s="44"/>
       <c r="C56" s="36"/>
@@ -8815,7 +8783,7 @@
       <c r="I56" s="36"/>
       <c r="J56" s="36"/>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57" s="44"/>
       <c r="B57" s="44"/>
       <c r="C57" s="36"/>
@@ -8827,12 +8795,12 @@
       <c r="I57" s="36"/>
       <c r="J57" s="36"/>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A58" s="39" t="s">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A58" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="B58" s="39"/>
-      <c r="C58" s="35"/>
+      <c r="B58" s="44"/>
+      <c r="C58" s="36"/>
       <c r="D58" s="36"/>
       <c r="E58" s="36"/>
       <c r="F58" s="36"/>
@@ -8840,13 +8808,16 @@
       <c r="H58" s="36"/>
       <c r="I58" s="36"/>
       <c r="J58" s="36"/>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A59" s="39" t="s">
+      <c r="K58" s="36"/>
+      <c r="L58" s="36"/>
+      <c r="M58" s="36"/>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A59" s="44" t="s">
         <v>58</v>
       </c>
-      <c r="B59" s="39"/>
-      <c r="C59" s="35"/>
+      <c r="B59" s="44"/>
+      <c r="C59" s="36"/>
       <c r="D59" s="36"/>
       <c r="E59" s="36"/>
       <c r="F59" s="36"/>
@@ -8854,14 +8825,17 @@
       <c r="H59" s="36"/>
       <c r="I59" s="36"/>
       <c r="J59" s="36"/>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A60" s="39" t="str">
+      <c r="K59" s="36"/>
+      <c r="L59" s="36"/>
+      <c r="M59" s="36"/>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A60" s="44" t="str">
         <f>CONCATENATE("OMSÆTNING = ",A6,"*",A89,"=",A6*A89)</f>
-        <v>OMSÆTNING = 50*30=1500</v>
-      </c>
-      <c r="B60" s="39"/>
-      <c r="C60" s="35"/>
+        <v>OMSÆTNING = 50*50=2500</v>
+      </c>
+      <c r="B60" s="44"/>
+      <c r="C60" s="36"/>
       <c r="D60" s="36"/>
       <c r="E60" s="36"/>
       <c r="F60" s="36"/>
@@ -8869,17 +8843,20 @@
       <c r="H60" s="36"/>
       <c r="I60" s="36"/>
       <c r="J60" s="36"/>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A61" s="39" t="str">
+      <c r="K60" s="36"/>
+      <c r="L60" s="36"/>
+      <c r="M60" s="36"/>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A61" s="44" t="str">
         <f>CONCATENATE("VE = ",B61)</f>
-        <v>VE = 38,4615384615385</v>
-      </c>
-      <c r="B61" s="39">
+        <v>VE = 48,0769230769231</v>
+      </c>
+      <c r="B61" s="44">
         <f>A80*(A6*0.5)+B6</f>
-        <v>38.461538461538467</v>
-      </c>
-      <c r="C61" s="35"/>
+        <v>48.07692307692308</v>
+      </c>
+      <c r="C61" s="36"/>
       <c r="D61" s="36"/>
       <c r="E61" s="36"/>
       <c r="F61" s="36"/>
@@ -8887,14 +8864,17 @@
       <c r="H61" s="36"/>
       <c r="I61" s="36"/>
       <c r="J61" s="36"/>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A62" s="39" t="str">
+      <c r="K61" s="36"/>
+      <c r="L61" s="36"/>
+      <c r="M61" s="36"/>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A62" s="44" t="str">
         <f>CONCATENATE("Maks. betalingsvillighed = ",B3,"kr.")</f>
-        <v>Maks. betalingsvillighed = 80kr.</v>
-      </c>
-      <c r="B62" s="39"/>
-      <c r="C62" s="35"/>
+        <v>Maks. betalingsvillighed = 100kr.</v>
+      </c>
+      <c r="B62" s="44"/>
+      <c r="C62" s="36"/>
       <c r="D62" s="36"/>
       <c r="E62" s="36"/>
       <c r="F62" s="36"/>
@@ -8902,14 +8882,17 @@
       <c r="H62" s="36"/>
       <c r="I62" s="36"/>
       <c r="J62" s="36"/>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A63" s="39" t="str">
+      <c r="K62" s="36"/>
+      <c r="L62" s="36"/>
+      <c r="M62" s="36"/>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A63" s="44" t="str">
         <f>CONCATENATE("Markedsmætning = ",-B3/A3,"Q")</f>
-        <v>Markedsmætning = 80Q</v>
-      </c>
-      <c r="B63" s="40"/>
-      <c r="C63" s="35"/>
+        <v>Markedsmætning = 100Q</v>
+      </c>
+      <c r="B63" s="45"/>
+      <c r="C63" s="36"/>
       <c r="D63" s="36"/>
       <c r="E63" s="36"/>
       <c r="F63" s="36"/>
@@ -8917,11 +8900,14 @@
       <c r="H63" s="36"/>
       <c r="I63" s="36"/>
       <c r="J63" s="36"/>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A64" s="39"/>
-      <c r="B64" s="39"/>
-      <c r="C64" s="35"/>
+      <c r="K63" s="36"/>
+      <c r="L63" s="36"/>
+      <c r="M63" s="36"/>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A64" s="44"/>
+      <c r="B64" s="44"/>
+      <c r="C64" s="36"/>
       <c r="D64" s="36"/>
       <c r="E64" s="36"/>
       <c r="F64" s="36"/>
@@ -8929,14 +8915,17 @@
       <c r="H64" s="36"/>
       <c r="I64" s="36"/>
       <c r="J64" s="36"/>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A65" s="39"/>
-      <c r="B65" s="39" t="str">
+      <c r="K64" s="36"/>
+      <c r="L64" s="36"/>
+      <c r="M64" s="36"/>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A65" s="44"/>
+      <c r="B65" s="44" t="str">
         <f>CONCATENATE("P = ",A3,"·Q + ",B3)</f>
-        <v>P = -1·Q + 80</v>
-      </c>
-      <c r="C65" s="35"/>
+        <v>P = -1·Q + 100</v>
+      </c>
+      <c r="C65" s="36"/>
       <c r="D65" s="36"/>
       <c r="E65" s="36"/>
       <c r="F65" s="36"/>
@@ -8944,16 +8933,19 @@
       <c r="H65" s="36"/>
       <c r="I65" s="36"/>
       <c r="J65" s="36"/>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A66" s="39">
+      <c r="K65" s="36"/>
+      <c r="L65" s="36"/>
+      <c r="M65" s="36"/>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A66" s="44">
         <v>0</v>
       </c>
-      <c r="B66" s="39">
+      <c r="B66" s="44">
         <f>B3</f>
-        <v>80</v>
-      </c>
-      <c r="C66" s="35"/>
+        <v>100</v>
+      </c>
+      <c r="C66" s="36"/>
       <c r="D66" s="36"/>
       <c r="E66" s="36"/>
       <c r="F66" s="36"/>
@@ -8961,16 +8953,19 @@
       <c r="H66" s="36"/>
       <c r="I66" s="36"/>
       <c r="J66" s="36"/>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A67" s="39">
+      <c r="K66" s="36"/>
+      <c r="L66" s="36"/>
+      <c r="M66" s="36"/>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A67" s="44">
         <f>-B3/A3</f>
-        <v>80</v>
-      </c>
-      <c r="B67" s="39">
+        <v>100</v>
+      </c>
+      <c r="B67" s="44">
         <v>0</v>
       </c>
-      <c r="C67" s="35"/>
+      <c r="C67" s="36"/>
       <c r="D67" s="36"/>
       <c r="E67" s="36"/>
       <c r="F67" s="36"/>
@@ -8978,14 +8973,17 @@
       <c r="H67" s="36"/>
       <c r="I67" s="36"/>
       <c r="J67" s="36"/>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A68" s="39"/>
-      <c r="B68" s="39" t="str">
+      <c r="K67" s="36"/>
+      <c r="L67" s="36"/>
+      <c r="M67" s="36"/>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A68" s="44"/>
+      <c r="B68" s="44" t="str">
         <f>CONCATENATE("GROMS = ",A3*2,"·m + ",B3)</f>
-        <v>GROMS = -2·m + 80</v>
-      </c>
-      <c r="C68" s="35"/>
+        <v>GROMS = -2·m + 100</v>
+      </c>
+      <c r="C68" s="36"/>
       <c r="D68" s="36"/>
       <c r="E68" s="36"/>
       <c r="F68" s="36"/>
@@ -8993,16 +8991,19 @@
       <c r="H68" s="36"/>
       <c r="I68" s="36"/>
       <c r="J68" s="36"/>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A69" s="39">
+      <c r="K68" s="36"/>
+      <c r="L68" s="36"/>
+      <c r="M68" s="36"/>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A69" s="44">
         <v>0</v>
       </c>
-      <c r="B69" s="39">
+      <c r="B69" s="44">
         <f>B3</f>
-        <v>80</v>
-      </c>
-      <c r="C69" s="35"/>
+        <v>100</v>
+      </c>
+      <c r="C69" s="36"/>
       <c r="D69" s="36"/>
       <c r="E69" s="36"/>
       <c r="F69" s="36"/>
@@ -9010,16 +9011,19 @@
       <c r="H69" s="36"/>
       <c r="I69" s="36"/>
       <c r="J69" s="36"/>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A70" s="39">
+      <c r="K69" s="36"/>
+      <c r="L69" s="36"/>
+      <c r="M69" s="36"/>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A70" s="44">
         <f>-B3/(2*A3)</f>
-        <v>40</v>
-      </c>
-      <c r="B70" s="39">
+        <v>50</v>
+      </c>
+      <c r="B70" s="44">
         <v>0</v>
       </c>
-      <c r="C70" s="35"/>
+      <c r="C70" s="36"/>
       <c r="D70" s="36"/>
       <c r="E70" s="36"/>
       <c r="F70" s="36"/>
@@ -9027,14 +9031,17 @@
       <c r="H70" s="36"/>
       <c r="I70" s="36"/>
       <c r="J70" s="36"/>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A71" s="39"/>
-      <c r="B71" s="39" t="str">
+      <c r="K70" s="36"/>
+      <c r="L70" s="36"/>
+      <c r="M70" s="36"/>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A71" s="44"/>
+      <c r="B71" s="44" t="str">
         <f>IF(A6="",CONCATENATE("GROMK = ",B6),CONCATENATE("GROMK = ",A6,"·m + ",B6))</f>
         <v xml:space="preserve">GROMK = 50·m + </v>
       </c>
-      <c r="C71" s="35"/>
+      <c r="C71" s="36"/>
       <c r="D71" s="36"/>
       <c r="E71" s="36"/>
       <c r="F71" s="36"/>
@@ -9042,16 +9049,19 @@
       <c r="H71" s="36"/>
       <c r="I71" s="36"/>
       <c r="J71" s="36"/>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A72" s="39">
+      <c r="K71" s="36"/>
+      <c r="L71" s="36"/>
+      <c r="M71" s="36"/>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A72" s="44">
         <v>0</v>
       </c>
-      <c r="B72" s="39">
+      <c r="B72" s="44">
         <f>B6</f>
         <v>0</v>
       </c>
-      <c r="C72" s="35"/>
+      <c r="C72" s="36"/>
       <c r="D72" s="36"/>
       <c r="E72" s="36"/>
       <c r="F72" s="36"/>
@@ -9059,17 +9069,20 @@
       <c r="H72" s="36"/>
       <c r="I72" s="36"/>
       <c r="J72" s="36"/>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A73" s="39">
+      <c r="K72" s="36"/>
+      <c r="L72" s="36"/>
+      <c r="M72" s="36"/>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A73" s="44">
         <f>A67</f>
-        <v>80</v>
-      </c>
-      <c r="B73" s="39">
+        <v>100</v>
+      </c>
+      <c r="B73" s="44">
         <f>A6*A67+B6</f>
-        <v>4000</v>
-      </c>
-      <c r="C73" s="35"/>
+        <v>5000</v>
+      </c>
+      <c r="C73" s="36"/>
       <c r="D73" s="36"/>
       <c r="E73" s="36"/>
       <c r="F73" s="36"/>
@@ -9078,14 +9091,16 @@
       <c r="I73" s="36"/>
       <c r="J73" s="36"/>
       <c r="K73" s="36"/>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A74" s="39"/>
-      <c r="B74" s="39" t="str">
+      <c r="L73" s="36"/>
+      <c r="M73" s="36"/>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A74" s="44"/>
+      <c r="B74" s="44" t="str">
         <f>IF(A8="","",CONCATENATE("Kapacitet = ",A8))</f>
         <v/>
       </c>
-      <c r="C74" s="35"/>
+      <c r="C74" s="36"/>
       <c r="D74" s="36"/>
       <c r="E74" s="36"/>
       <c r="F74" s="36"/>
@@ -9094,17 +9109,19 @@
       <c r="I74" s="36"/>
       <c r="J74" s="36"/>
       <c r="K74" s="36"/>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A75" s="39" t="str">
+      <c r="L74" s="36"/>
+      <c r="M74" s="36"/>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A75" s="44" t="str">
         <f>IF(A8="","",A8)</f>
         <v/>
       </c>
-      <c r="B75" s="39" t="str">
+      <c r="B75" s="44" t="str">
         <f>IF(A8="","",0)</f>
         <v/>
       </c>
-      <c r="C75" s="35"/>
+      <c r="C75" s="36"/>
       <c r="D75" s="36"/>
       <c r="E75" s="36"/>
       <c r="F75" s="36"/>
@@ -9113,17 +9130,19 @@
       <c r="I75" s="36"/>
       <c r="J75" s="36"/>
       <c r="K75" s="36"/>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A76" s="39" t="str">
+      <c r="L75" s="36"/>
+      <c r="M75" s="36"/>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A76" s="44" t="str">
         <f>IF(A8="","",A8)</f>
         <v/>
       </c>
-      <c r="B76" s="39" t="str">
+      <c r="B76" s="44" t="str">
         <f>IF(A8="","",B3)</f>
         <v/>
       </c>
-      <c r="C76" s="35"/>
+      <c r="C76" s="36"/>
       <c r="D76" s="36"/>
       <c r="E76" s="36"/>
       <c r="F76" s="36"/>
@@ -9132,13 +9151,15 @@
       <c r="I76" s="36"/>
       <c r="J76" s="36"/>
       <c r="K76" s="36"/>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A77" s="39" t="s">
+      <c r="L76" s="36"/>
+      <c r="M76" s="36"/>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A77" s="44" t="s">
         <v>56</v>
       </c>
-      <c r="B77" s="39"/>
-      <c r="C77" s="35"/>
+      <c r="B77" s="44"/>
+      <c r="C77" s="36"/>
       <c r="D77" s="36"/>
       <c r="E77" s="36"/>
       <c r="F77" s="36"/>
@@ -9147,14 +9168,16 @@
       <c r="I77" s="36"/>
       <c r="J77" s="36"/>
       <c r="K77" s="36"/>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A78" s="39">
+      <c r="L77" s="36"/>
+      <c r="M77" s="36"/>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A78" s="44">
         <f>(B6-B3)/(A3*2-A6)</f>
-        <v>1.5384615384615385</v>
-      </c>
-      <c r="B78" s="39"/>
-      <c r="C78" s="35"/>
+        <v>1.9230769230769231</v>
+      </c>
+      <c r="B78" s="44"/>
+      <c r="C78" s="36"/>
       <c r="D78" s="36"/>
       <c r="E78" s="36"/>
       <c r="F78" s="36"/>
@@ -9163,15 +9186,17 @@
       <c r="I78" s="36"/>
       <c r="J78" s="36"/>
       <c r="K78" s="36"/>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A79" s="39" t="s">
+      <c r="L78" s="36"/>
+      <c r="M78" s="36"/>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A79" s="44" t="s">
         <v>55</v>
       </c>
-      <c r="B79" s="39" t="s">
+      <c r="B79" s="44" t="s">
         <v>57</v>
       </c>
-      <c r="C79" s="35"/>
+      <c r="C79" s="36"/>
       <c r="D79" s="36"/>
       <c r="E79" s="36"/>
       <c r="F79" s="36"/>
@@ -9180,17 +9205,19 @@
       <c r="I79" s="36"/>
       <c r="J79" s="36"/>
       <c r="K79" s="36"/>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A80" s="39">
+      <c r="L79" s="36"/>
+      <c r="M79" s="36"/>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A80" s="44">
         <f>IF(A8&lt;&gt;"",MIN(A78,A8),A78)</f>
-        <v>1.5384615384615385</v>
-      </c>
-      <c r="B80" s="39">
+        <v>1.9230769230769231</v>
+      </c>
+      <c r="B80" s="44">
         <f>A3*A80+B3</f>
-        <v>78.461538461538467</v>
-      </c>
-      <c r="C80" s="35"/>
+        <v>98.07692307692308</v>
+      </c>
+      <c r="C80" s="36"/>
       <c r="D80" s="36"/>
       <c r="E80" s="36"/>
       <c r="F80" s="36"/>
@@ -9199,14 +9226,16 @@
       <c r="I80" s="36"/>
       <c r="J80" s="36"/>
       <c r="K80" s="36"/>
-    </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A81" s="39"/>
-      <c r="B81" s="39" t="str">
+      <c r="L80" s="36"/>
+      <c r="M80" s="36"/>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A81" s="44"/>
+      <c r="B81" s="44" t="str">
         <f>IF(A6="",CONCATENATE("VE = ",B6),CONCATENATE("VE = ",A6*0.5,"·m + ",B6))</f>
         <v xml:space="preserve">VE = 25·m + </v>
       </c>
-      <c r="C81" s="35"/>
+      <c r="C81" s="36"/>
       <c r="D81" s="36"/>
       <c r="E81" s="36"/>
       <c r="F81" s="36"/>
@@ -9215,16 +9244,18 @@
       <c r="I81" s="36"/>
       <c r="J81" s="36"/>
       <c r="K81" s="36"/>
-    </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A82" s="39">
+      <c r="L81" s="36"/>
+      <c r="M81" s="36"/>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A82" s="44">
         <v>0</v>
       </c>
-      <c r="B82" s="39">
+      <c r="B82" s="44">
         <f>B6</f>
         <v>0</v>
       </c>
-      <c r="C82" s="35"/>
+      <c r="C82" s="36"/>
       <c r="D82" s="36"/>
       <c r="E82" s="36"/>
       <c r="F82" s="36"/>
@@ -9233,17 +9264,19 @@
       <c r="I82" s="36"/>
       <c r="J82" s="36"/>
       <c r="K82" s="36"/>
-    </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A83" s="39">
+      <c r="L82" s="36"/>
+      <c r="M82" s="36"/>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A83" s="44">
         <f>A67</f>
-        <v>80</v>
-      </c>
-      <c r="B83" s="39">
+        <v>100</v>
+      </c>
+      <c r="B83" s="44">
         <f>A67*(A6*0.5)+B6</f>
-        <v>2000</v>
-      </c>
-      <c r="C83" s="35"/>
+        <v>2500</v>
+      </c>
+      <c r="C83" s="36"/>
       <c r="D83" s="36"/>
       <c r="E83" s="36"/>
       <c r="F83" s="36"/>
@@ -9252,14 +9285,16 @@
       <c r="I83" s="36"/>
       <c r="J83" s="36"/>
       <c r="K83" s="36"/>
-    </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A84" s="39"/>
-      <c r="B84" s="39" t="str">
-        <f>CONCATENATE("Pris = ",A6)</f>
-        <v>Pris = 50</v>
-      </c>
-      <c r="C84" s="35"/>
+      <c r="L83" s="36"/>
+      <c r="M83" s="36"/>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A84" s="44"/>
+      <c r="B84" s="44" t="str">
+        <f>CONCATENATE("Pris = ",A6,"kr. Elasticiteten er ",A98,". Når prisen sænkes med 1%, stiger afsætningen med ",-A98,"%."," Efterspørgslen er",IF(A98&lt;-1," elastisk",IF(A98=-1," neutralelastisk"," uelastisk")))</f>
+        <v>Pris = 50kr. Elasticiteten er -1. Når prisen sænkes med 1%, stiger afsætningen med 1%. Efterspørgslen er neutralelastisk</v>
+      </c>
+      <c r="C84" s="36"/>
       <c r="D84" s="36"/>
       <c r="E84" s="36"/>
       <c r="F84" s="36"/>
@@ -9268,16 +9303,18 @@
       <c r="I84" s="36"/>
       <c r="J84" s="36"/>
       <c r="K84" s="36"/>
-    </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A85" s="39">
+      <c r="L84" s="36"/>
+      <c r="M84" s="36"/>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A85" s="44">
         <v>0</v>
       </c>
-      <c r="B85" s="39">
+      <c r="B85" s="44">
         <f>A6</f>
         <v>50</v>
       </c>
-      <c r="C85" s="35"/>
+      <c r="C85" s="36"/>
       <c r="D85" s="36"/>
       <c r="E85" s="36"/>
       <c r="F85" s="36"/>
@@ -9286,17 +9323,19 @@
       <c r="I85" s="36"/>
       <c r="J85" s="36"/>
       <c r="K85" s="36"/>
-    </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A86" s="39">
+      <c r="L85" s="36"/>
+      <c r="M85" s="36"/>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A86" s="44">
         <f>(A6-B3)/A3</f>
-        <v>30</v>
-      </c>
-      <c r="B86" s="39">
+        <v>50</v>
+      </c>
+      <c r="B86" s="44">
         <f>A6</f>
         <v>50</v>
       </c>
-      <c r="C86" s="35"/>
+      <c r="C86" s="36"/>
       <c r="D86" s="36"/>
       <c r="E86" s="36"/>
       <c r="F86" s="36"/>
@@ -9305,14 +9344,16 @@
       <c r="I86" s="36"/>
       <c r="J86" s="36"/>
       <c r="K86" s="36"/>
-    </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A87" s="39"/>
-      <c r="B87" s="39" t="str">
+      <c r="L86" s="36"/>
+      <c r="M86" s="36"/>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A87" s="44"/>
+      <c r="B87" s="44" t="str">
         <f>CONCATENATE("Mængde = ",(A6-B3)/A3)</f>
-        <v>Mængde = 30</v>
-      </c>
-      <c r="C87" s="35"/>
+        <v>Mængde = 50</v>
+      </c>
+      <c r="C87" s="36"/>
       <c r="D87" s="36"/>
       <c r="E87" s="36"/>
       <c r="F87" s="36"/>
@@ -9321,16 +9362,18 @@
       <c r="I87" s="36"/>
       <c r="J87" s="36"/>
       <c r="K87" s="36"/>
-    </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A88" s="39">
+      <c r="L87" s="36"/>
+      <c r="M87" s="36"/>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A88" s="44">
         <f>(A6-B3)/A3</f>
-        <v>30</v>
-      </c>
-      <c r="B88" s="39">
+        <v>50</v>
+      </c>
+      <c r="B88" s="44">
         <v>0</v>
       </c>
-      <c r="C88" s="35"/>
+      <c r="C88" s="36"/>
       <c r="D88" s="36"/>
       <c r="E88" s="36"/>
       <c r="F88" s="36"/>
@@ -9339,17 +9382,19 @@
       <c r="I88" s="36"/>
       <c r="J88" s="36"/>
       <c r="K88" s="36"/>
-    </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A89" s="39">
+      <c r="L88" s="36"/>
+      <c r="M88" s="36"/>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A89" s="44">
         <f>(A6-B3)/A3</f>
-        <v>30</v>
-      </c>
-      <c r="B89" s="39">
+        <v>50</v>
+      </c>
+      <c r="B89" s="44">
         <f>A6</f>
         <v>50</v>
       </c>
-      <c r="C89" s="35"/>
+      <c r="C89" s="36"/>
       <c r="D89" s="36"/>
       <c r="E89" s="36"/>
       <c r="F89" s="36"/>
@@ -9358,11 +9403,16 @@
       <c r="I89" s="36"/>
       <c r="J89" s="36"/>
       <c r="K89" s="36"/>
-    </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A90" s="35"/>
-      <c r="B90" s="35"/>
-      <c r="C90" s="35"/>
+      <c r="L89" s="36"/>
+      <c r="M89" s="36"/>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A90" s="36" t="str">
+        <f>CONCATENATE("Markedsmætning = ",-B3/A3," Q")</f>
+        <v>Markedsmætning = 100 Q</v>
+      </c>
+      <c r="B90" s="36"/>
+      <c r="C90" s="36"/>
       <c r="D90" s="36"/>
       <c r="E90" s="36"/>
       <c r="F90" s="36"/>
@@ -9371,14 +9421,13 @@
       <c r="I90" s="36"/>
       <c r="J90" s="36"/>
       <c r="K90" s="36"/>
-    </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A91" s="35" t="str">
-        <f>CONCATENATE("Markedsmætning = ",-B3/A3," Q")</f>
-        <v>Markedsmætning = 80 Q</v>
-      </c>
-      <c r="B91" s="35"/>
-      <c r="C91" s="35"/>
+      <c r="L90" s="36"/>
+      <c r="M90" s="36"/>
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A91" s="36"/>
+      <c r="B91" s="36"/>
+      <c r="C91" s="36"/>
       <c r="D91" s="36"/>
       <c r="E91" s="36"/>
       <c r="F91" s="36"/>
@@ -9388,15 +9437,15 @@
       <c r="J91" s="36"/>
       <c r="K91" s="36"/>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A92" s="35">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A92" s="36">
         <f>-B3/A3</f>
-        <v>80</v>
-      </c>
-      <c r="B92" s="35">
+        <v>100</v>
+      </c>
+      <c r="B92" s="36">
         <v>0</v>
       </c>
-      <c r="C92" s="35"/>
+      <c r="C92" s="36"/>
       <c r="D92" s="36"/>
       <c r="E92" s="36"/>
       <c r="F92" s="36"/>
@@ -9406,13 +9455,13 @@
       <c r="J92" s="36"/>
       <c r="K92" s="36"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A93" s="35" t="str">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A93" s="36" t="str">
         <f>CONCATENATE("Maks. betalingsvillighed = ",B3," kr.")</f>
-        <v>Maks. betalingsvillighed = 80 kr.</v>
-      </c>
-      <c r="B93" s="35"/>
-      <c r="C93" s="35"/>
+        <v>Maks. betalingsvillighed = 100 kr.</v>
+      </c>
+      <c r="B93" s="36"/>
+      <c r="C93" s="36"/>
       <c r="D93" s="36"/>
       <c r="E93" s="36"/>
       <c r="F93" s="36"/>
@@ -9422,15 +9471,15 @@
       <c r="J93" s="36"/>
       <c r="K93" s="36"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A94" s="35">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A94" s="36">
         <v>0</v>
       </c>
-      <c r="B94" s="35">
+      <c r="B94" s="36">
         <f>B3</f>
-        <v>80</v>
-      </c>
-      <c r="C94" s="35"/>
+        <v>100</v>
+      </c>
+      <c r="C94" s="36"/>
       <c r="D94" s="36"/>
       <c r="E94" s="36"/>
       <c r="F94" s="36"/>
@@ -9440,13 +9489,13 @@
       <c r="J94" s="36"/>
       <c r="K94" s="36"/>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A95" s="35" t="str">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A95" s="36" t="str">
         <f>CONCATENATE("Maks. omsætning = ",B3/2,"*",(B3/2-B3)/A3," = ",B3/2*(B3/2-B3)/A3," kr.")</f>
-        <v>Maks. omsætning = 40*40 = 1600 kr.</v>
-      </c>
-      <c r="B95" s="35"/>
-      <c r="C95" s="35"/>
+        <v>Maks. omsætning = 50*50 = 2500 kr.</v>
+      </c>
+      <c r="B95" s="36"/>
+      <c r="C95" s="36"/>
       <c r="D95" s="36"/>
       <c r="E95" s="36"/>
       <c r="F95" s="36"/>
@@ -9456,16 +9505,16 @@
       <c r="J95" s="36"/>
       <c r="K95" s="36"/>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A96" s="35">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A96" s="36">
         <f>(B3/2-B3)/A3</f>
-        <v>40</v>
-      </c>
-      <c r="B96" s="35">
+        <v>50</v>
+      </c>
+      <c r="B96" s="36">
         <f>B3/2</f>
-        <v>40</v>
-      </c>
-      <c r="C96" s="35"/>
+        <v>50</v>
+      </c>
+      <c r="C96" s="36"/>
       <c r="D96" s="36"/>
       <c r="E96" s="36"/>
       <c r="F96" s="36"/>
@@ -9476,7 +9525,9 @@
       <c r="K96" s="36"/>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A97" s="36"/>
+      <c r="A97" s="36" t="s">
+        <v>87</v>
+      </c>
       <c r="B97" s="36"/>
       <c r="C97" s="36"/>
       <c r="D97" s="36"/>
@@ -9489,7 +9540,10 @@
       <c r="K97" s="36"/>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A98" s="36"/>
+      <c r="A98" s="36">
+        <f>ROUND(-A6/(B3-A6),2)</f>
+        <v>-1</v>
+      </c>
       <c r="B98" s="36"/>
       <c r="C98" s="36"/>
       <c r="D98" s="36"/>
@@ -9727,7 +9781,7 @@
   <dimension ref="A1:K110"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9752,10 +9806,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="62">
-        <v>-0.01</v>
+        <v>-0.02</v>
       </c>
       <c r="B3" s="62">
-        <v>2000</v>
+        <v>300</v>
       </c>
       <c r="E3" s="37"/>
     </row>
@@ -9776,7 +9830,9 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="26"/>
-      <c r="B6" s="26"/>
+      <c r="B6" s="26">
+        <v>0</v>
+      </c>
       <c r="E6" s="37"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -9948,7 +10004,7 @@
       </c>
       <c r="B58" s="39">
         <f>B80</f>
-        <v>1000</v>
+        <v>150</v>
       </c>
       <c r="C58" s="35"/>
       <c r="D58" s="35"/>
@@ -9962,7 +10018,7 @@
       </c>
       <c r="B59" s="39">
         <f>A80</f>
-        <v>100000</v>
+        <v>7500</v>
       </c>
       <c r="C59" s="35"/>
       <c r="D59" s="35"/>
@@ -9973,11 +10029,11 @@
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="39" t="str">
         <f>CONCATENATE("OMSÆTNING = ",B60)</f>
-        <v>OMSÆTNING = 100000000</v>
+        <v>OMSÆTNING = 1125000</v>
       </c>
       <c r="B60" s="39">
         <f>B58*B59</f>
-        <v>100000000</v>
+        <v>1125000</v>
       </c>
       <c r="C60" s="35"/>
       <c r="D60" s="35"/>
@@ -10018,11 +10074,11 @@
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" s="39" t="str">
         <f>CONCATENATE("DB = ",B63)</f>
-        <v>DB = 100000000</v>
+        <v>DB = 1125000</v>
       </c>
       <c r="B63" s="40">
         <f>B60-B62</f>
-        <v>100000000</v>
+        <v>1125000</v>
       </c>
       <c r="C63" s="35"/>
       <c r="D63" s="35"/>
@@ -10043,7 +10099,7 @@
       <c r="A65" s="39"/>
       <c r="B65" s="39" t="str">
         <f>CONCATENATE("P = ",A3,"·m + ",B3)</f>
-        <v>P = -0,01·m + 2000</v>
+        <v>P = -0,02·m + 300</v>
       </c>
       <c r="C65" s="35"/>
       <c r="D65" s="35"/>
@@ -10057,7 +10113,7 @@
       </c>
       <c r="B66" s="39">
         <f>B3</f>
-        <v>2000</v>
+        <v>300</v>
       </c>
       <c r="C66" s="35"/>
       <c r="D66" s="35"/>
@@ -10068,7 +10124,7 @@
     <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67" s="39">
         <f>-B3/A3</f>
-        <v>200000</v>
+        <v>15000</v>
       </c>
       <c r="B67" s="39">
         <v>0</v>
@@ -10083,7 +10139,7 @@
       <c r="A68" s="39"/>
       <c r="B68" s="39" t="str">
         <f>CONCATENATE("GROMS = ",A3*2,"·m + ",B3)</f>
-        <v>GROMS = -0,02·m + 2000</v>
+        <v>GROMS = -0,04·m + 300</v>
       </c>
       <c r="C68" s="35"/>
       <c r="D68" s="35"/>
@@ -10097,7 +10153,7 @@
       </c>
       <c r="B69" s="39">
         <f>B3</f>
-        <v>2000</v>
+        <v>300</v>
       </c>
       <c r="C69" s="35"/>
       <c r="D69" s="35"/>
@@ -10108,7 +10164,7 @@
     <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70" s="39">
         <f>-B3/(2*A3)</f>
-        <v>100000</v>
+        <v>7500</v>
       </c>
       <c r="B70" s="39">
         <v>0</v>
@@ -10123,7 +10179,7 @@
       <c r="A71" s="39"/>
       <c r="B71" s="39" t="str">
         <f>IF(A6="",CONCATENATE("GROMK = ",B6),CONCATENATE("GROMK = ",A6,"·m + ",B6))</f>
-        <v xml:space="preserve">GROMK = </v>
+        <v>GROMK = 0</v>
       </c>
       <c r="C71" s="35"/>
       <c r="D71" s="35"/>
@@ -10148,7 +10204,7 @@
     <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73" s="39">
         <f>A67</f>
-        <v>200000</v>
+        <v>15000</v>
       </c>
       <c r="B73" s="39">
         <f>A6*A67+B6</f>
@@ -10236,7 +10292,7 @@
     <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78" s="39">
         <f>(B6-B3)/(A3*2-A6)</f>
-        <v>100000</v>
+        <v>7500</v>
       </c>
       <c r="B78" s="39"/>
       <c r="C78" s="35"/>
@@ -10269,11 +10325,11 @@
     <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80" s="39">
         <f>IF(A8&lt;&gt;"",MIN(A78,A8),A78)</f>
-        <v>100000</v>
+        <v>7500</v>
       </c>
       <c r="B80" s="39">
         <f>A3*A80+B3</f>
-        <v>1000</v>
+        <v>150</v>
       </c>
       <c r="C80" s="35"/>
       <c r="D80" s="35"/>
@@ -10289,7 +10345,7 @@
       <c r="A81" s="39"/>
       <c r="B81" s="39" t="str">
         <f>IF(A6="",CONCATENATE("VE = ",B6),CONCATENATE("VE = ",A6*0.5,"·m + ",B6))</f>
-        <v xml:space="preserve">VE = </v>
+        <v>VE = 0</v>
       </c>
       <c r="C81" s="35"/>
       <c r="D81" s="35"/>
@@ -10322,7 +10378,7 @@
     <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83" s="39">
         <f>A67</f>
-        <v>200000</v>
+        <v>15000</v>
       </c>
       <c r="B83" s="39">
         <f>A67*(A6*0.5)+B6</f>
@@ -10342,7 +10398,7 @@
       <c r="A84" s="39"/>
       <c r="B84" s="39" t="str">
         <f>CONCATENATE("Optimal pris = ",B80)</f>
-        <v>Optimal pris = 1000</v>
+        <v>Optimal pris = 150</v>
       </c>
       <c r="C84" s="35"/>
       <c r="D84" s="35"/>
@@ -10360,7 +10416,7 @@
       </c>
       <c r="B85" s="39">
         <f>B80</f>
-        <v>1000</v>
+        <v>150</v>
       </c>
       <c r="C85" s="35"/>
       <c r="D85" s="35"/>
@@ -10375,11 +10431,11 @@
     <row r="86" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A86" s="39">
         <f>A80</f>
-        <v>100000</v>
+        <v>7500</v>
       </c>
       <c r="B86" s="39">
         <f>B80</f>
-        <v>1000</v>
+        <v>150</v>
       </c>
       <c r="C86" s="35"/>
       <c r="D86" s="35"/>
@@ -10395,7 +10451,7 @@
       <c r="A87" s="39"/>
       <c r="B87" s="39" t="str">
         <f>CONCATENATE("Optimal mængde = ",A80)</f>
-        <v>Optimal mængde = 100000</v>
+        <v>Optimal mængde = 7500</v>
       </c>
       <c r="C87" s="35"/>
       <c r="D87" s="35"/>
@@ -10410,7 +10466,7 @@
     <row r="88" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A88" s="39">
         <f>A80</f>
-        <v>100000</v>
+        <v>7500</v>
       </c>
       <c r="B88" s="39">
         <v>0</v>
@@ -10428,11 +10484,11 @@
     <row r="89" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A89" s="39">
         <f>A80</f>
-        <v>100000</v>
+        <v>7500</v>
       </c>
       <c r="B89" s="39">
         <f>B80</f>
-        <v>1000</v>
+        <v>150</v>
       </c>
       <c r="C89" s="35"/>
       <c r="D89" s="35"/>

</xml_diff>